<commit_message>
Se solucionó error semántico
</commit_message>
<xml_diff>
--- a/claves.xlsx
+++ b/claves.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmend\Desktop\selenium\bot_descarga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FB4E4B-DE64-41A9-A5F5-C9A5E8C82C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFA9146-33C9-420B-8779-1D80504527AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CF8CC744-D4E2-4D21-B3D7-A0FA736523ED}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <t>cuit</t>
   </si>
   <si>
-    <t>ClavePrueba1</t>
+    <t>clave01</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC6B368-C774-42CF-BB2E-074217992A11}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -422,7 +424,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>20222222223</v>
+        <v>20000000001</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Se modifican opciones del navegador
</commit_message>
<xml_diff>
--- a/claves.xlsx
+++ b/claves.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmend\Desktop\selenium\bot_descarga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFA9146-33C9-420B-8779-1D80504527AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD48FABD-B204-438E-B45F-C09A36B4BD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CF8CC744-D4E2-4D21-B3D7-A0FA736523ED}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <t>cuit</t>
   </si>
   <si>
-    <t>clave01</t>
+    <t>clave1234</t>
   </si>
 </sst>
 </file>
@@ -77,15 +77,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -402,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC6B368-C774-42CF-BB2E-074217992A11}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,88 +412,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>20000000001</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se establecen tiempos de espera aleatorios
</commit_message>
<xml_diff>
--- a/claves.xlsx
+++ b/claves.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmend\Desktop\selenium\bot_descarga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD48FABD-B204-438E-B45F-C09A36B4BD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4D91C9-23FE-4D5D-96F5-E1505F8DF838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CF8CC744-D4E2-4D21-B3D7-A0FA736523ED}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <t>cuit</t>
   </si>
   <si>
-    <t>clave1234</t>
+    <t>clave123</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se realizan cambios por modificaciones en la web de AFIP
</commit_message>
<xml_diff>
--- a/claves.xlsx
+++ b/claves.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmend\Desktop\selenium\bot_descarga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\bot_descarga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4D91C9-23FE-4D5D-96F5-E1505F8DF838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A926A6D7-3DAD-46E6-B12B-D58F6F4E48C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CF8CC744-D4E2-4D21-B3D7-A0FA736523ED}"/>
   </bookViews>
@@ -401,9 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC6B368-C774-42CF-BB2E-074217992A11}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>